<commit_message>
week 2 : 1068 트리 복습
지역변수 명 조심
</commit_message>
<xml_diff>
--- a/큰돌의 터전_틀린문제_복습양식.xlsx
+++ b/큰돌의 터전_틀린문제_복습양식.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyunwoo\source\repos\c++알고리즘\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760E3B1E-A09F-4538-A1A0-D40D6224B5DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD4DF2C-DF89-4F94-905A-E6D1F49EBDA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4128" yWindow="1812" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -465,7 +465,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -584,6 +584,9 @@
       <c r="C8" s="3">
         <v>45901</v>
       </c>
+      <c r="D8" s="3">
+        <v>45902</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
week 3 : 3197 백조의 호수
경계면 녹이기
</commit_message>
<xml_diff>
--- a/큰돌의 터전_틀린문제_복습양식.xlsx
+++ b/큰돌의 터전_틀린문제_복습양식.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyunwoo\source\repos\c++알고리즘\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A066D9-1C97-4C5D-BD61-85C0A8E9774E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6752EEE-866D-430F-9DA8-6B62A8DCD89C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4128" yWindow="1812" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>번호</t>
   </si>
@@ -72,6 +72,18 @@
   </si>
   <si>
     <t>불</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>숨바꼭질 5</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>괄호추가하기</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>백조의 호수</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -465,11 +477,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -603,6 +615,39 @@
         <v>45903</v>
       </c>
     </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A10">
+        <v>17071</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="3">
+        <v>45904</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A11">
+        <v>16637</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="3">
+        <v>45904</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A12">
+        <v>3197</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="3">
+        <v>45905</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
week 3 : 1189
visited가 아닌 원하는 장소 도달할때 기준
</commit_message>
<xml_diff>
--- a/큰돌의 터전_틀린문제_복습양식.xlsx
+++ b/큰돌의 터전_틀린문제_복습양식.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyunwoo\source\repos\c++알고리즘\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6752EEE-866D-430F-9DA8-6B62A8DCD89C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B27366F-B4A3-423B-9316-15208DBEA656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4128" yWindow="1812" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>번호</t>
   </si>
@@ -84,6 +84,14 @@
   </si>
   <si>
     <t>백조의 호수</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>사다리조작</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>꽃길</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -477,11 +485,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -648,6 +656,28 @@
         <v>45905</v>
       </c>
     </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A13">
+        <v>15684</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="3">
+        <v>45905</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A14">
+        <v>14620</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="3">
+        <v>45909</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
week 4 : 1987 알파벳_bitmasking
원하는 부분에 비트를 |해서 매개변수로 넘긴다면 visited[]=1 go() visited[]=0과 같은효과
</commit_message>
<xml_diff>
--- a/큰돌의 터전_틀린문제_복습양식.xlsx
+++ b/큰돌의 터전_틀린문제_복습양식.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyunwoo\source\repos\c++알고리즘\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B27366F-B4A3-423B-9316-15208DBEA656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01DF069B-45FF-45B6-AD67-DC4563CCEA65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4128" yWindow="1812" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>번호</t>
   </si>
@@ -92,6 +92,10 @@
   </si>
   <si>
     <t>꽃길</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>알파벳(비트마스킹)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -485,11 +489,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -678,6 +682,17 @@
         <v>45909</v>
       </c>
     </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A15">
+        <v>1987</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="3">
+        <v>45910</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
week 4 : 14890 경사로 문제
비트마스킹에 집착하지말것, 경계범위를 잘 신경쓸것
</commit_message>
<xml_diff>
--- a/큰돌의 터전_틀린문제_복습양식.xlsx
+++ b/큰돌의 터전_틀린문제_복습양식.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyunwoo\source\repos\c++알고리즘\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01DF069B-45FF-45B6-AD67-DC4563CCEA65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2290561-4931-4E73-89D5-F5CFD5A1A03B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4128" yWindow="1812" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>번호</t>
   </si>
@@ -96,6 +96,10 @@
   </si>
   <si>
     <t>알파벳(비트마스킹)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>경사로</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -489,11 +493,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -693,6 +697,17 @@
         <v>45910</v>
       </c>
     </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A16">
+        <v>14890</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="3">
+        <v>45910</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
week 4 : 1062
가르침 문제, 또한 부분집합의 경우 &를 통해 쉽게 분별가능:
</commit_message>
<xml_diff>
--- a/큰돌의 터전_틀린문제_복습양식.xlsx
+++ b/큰돌의 터전_틀린문제_복습양식.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyunwoo\source\repos\c++알고리즘\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2290561-4931-4E73-89D5-F5CFD5A1A03B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE78895-ACD4-401B-949D-9A7BE2D7BE82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4128" yWindow="1812" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>번호</t>
   </si>
@@ -100,6 +100,10 @@
   </si>
   <si>
     <t>경사로</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>가르침</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -493,11 +497,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -708,6 +712,17 @@
         <v>45910</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A17">
+        <v>1062</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="3">
+        <v>45910</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>